<commit_message>
FIX: Updated the excel spread sheet,
Question 54's weighting has been reversed

The tab color on Question 45 has been corrected.
</commit_message>
<xml_diff>
--- a/survey_data/SurveySummary_08192016.xlsx
+++ b/survey_data/SurveySummary_08192016.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="100" windowWidth="33240" windowHeight="19200" tabRatio="768" firstSheet="5" activeTab="8"/>
+    <workbookView xWindow="240" yWindow="100" windowWidth="33240" windowHeight="19200" tabRatio="768" firstSheet="24" activeTab="36"/>
   </bookViews>
   <sheets>
     <sheet name="Survey Tree Map" sheetId="56" r:id="rId1"/>
@@ -2062,11 +2062,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2079823976"/>
-        <c:axId val="-2080054952"/>
+        <c:axId val="-2073640872"/>
+        <c:axId val="-2073657736"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2079823976"/>
+        <c:axId val="-2073640872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2101,7 +2101,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2080054952"/>
+        <c:crossAx val="-2073657736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2111,7 +2111,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2080054952"/>
+        <c:axId val="-2073657736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2156,7 +2156,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2079823976"/>
+        <c:crossAx val="-2073640872"/>
         <c:crossesAt val="1.0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2865,11 +2865,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2092933080"/>
-        <c:axId val="-2075862952"/>
+        <c:axId val="-2073939736"/>
+        <c:axId val="-2073943128"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2092933080"/>
+        <c:axId val="-2073939736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2904,7 +2904,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2075862952"/>
+        <c:crossAx val="-2073943128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2914,7 +2914,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2075862952"/>
+        <c:axId val="-2073943128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2959,7 +2959,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2092933080"/>
+        <c:crossAx val="-2073939736"/>
         <c:crossesAt val="1.0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5208,11 +5208,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2081853208"/>
-        <c:axId val="-2081909496"/>
+        <c:axId val="-2085839896"/>
+        <c:axId val="-2085866456"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2081853208"/>
+        <c:axId val="-2085839896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5247,7 +5247,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2081909496"/>
+        <c:crossAx val="-2085866456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5257,7 +5257,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2081909496"/>
+        <c:axId val="-2085866456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5302,7 +5302,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2081853208"/>
+        <c:crossAx val="-2085839896"/>
         <c:crossesAt val="1.0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5545,11 +5545,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2085867032"/>
-        <c:axId val="-2080293000"/>
+        <c:axId val="-2086320968"/>
+        <c:axId val="-2086364184"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2085867032"/>
+        <c:axId val="-2086320968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5584,7 +5584,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2080293000"/>
+        <c:crossAx val="-2086364184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5594,7 +5594,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2080293000"/>
+        <c:axId val="-2086364184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5639,7 +5639,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2085867032"/>
+        <c:crossAx val="-2086320968"/>
         <c:crossesAt val="1.0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5822,11 +5822,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2096040632"/>
-        <c:axId val="-2086365416"/>
+        <c:axId val="-2086496440"/>
+        <c:axId val="-2086503704"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2096040632"/>
+        <c:axId val="-2086496440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5861,7 +5861,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2086365416"/>
+        <c:crossAx val="-2086503704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5871,7 +5871,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2086365416"/>
+        <c:axId val="-2086503704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5916,7 +5916,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2096040632"/>
+        <c:crossAx val="-2086496440"/>
         <c:crossesAt val="1.0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6386,11 +6386,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2076630808"/>
-        <c:axId val="-2076607880"/>
+        <c:axId val="-2087289720"/>
+        <c:axId val="-2087102792"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2076630808"/>
+        <c:axId val="-2087289720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6425,7 +6425,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2076607880"/>
+        <c:crossAx val="-2087102792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6435,7 +6435,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2076607880"/>
+        <c:axId val="-2087102792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6480,7 +6480,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2076630808"/>
+        <c:crossAx val="-2087289720"/>
         <c:crossesAt val="1.0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8580,11 +8580,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2079347640"/>
-        <c:axId val="-2080064328"/>
+        <c:axId val="-2090134440"/>
+        <c:axId val="-2082330056"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2079347640"/>
+        <c:axId val="-2090134440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8619,7 +8619,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2080064328"/>
+        <c:crossAx val="-2082330056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8629,7 +8629,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2080064328"/>
+        <c:axId val="-2082330056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8674,7 +8674,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2079347640"/>
+        <c:crossAx val="-2090134440"/>
         <c:crossesAt val="1.0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8917,11 +8917,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2082123448"/>
-        <c:axId val="-2082120024"/>
+        <c:axId val="-2087633896"/>
+        <c:axId val="-2081841944"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2082123448"/>
+        <c:axId val="-2087633896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8956,7 +8956,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2082120024"/>
+        <c:crossAx val="-2081841944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8966,7 +8966,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2082120024"/>
+        <c:axId val="-2081841944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9011,7 +9011,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2082123448"/>
+        <c:crossAx val="-2087633896"/>
         <c:crossesAt val="1.0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9194,11 +9194,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2082079320"/>
-        <c:axId val="-2082075928"/>
+        <c:axId val="-2082378664"/>
+        <c:axId val="-2082387976"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2082079320"/>
+        <c:axId val="-2082378664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9233,7 +9233,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2082075928"/>
+        <c:crossAx val="-2082387976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9243,7 +9243,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2082075928"/>
+        <c:axId val="-2082387976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9288,7 +9288,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2082079320"/>
+        <c:crossAx val="-2082378664"/>
         <c:crossesAt val="1.0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9731,19 +9731,19 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>3.428571428571428</c:v>
+                  <c:v>2.571428571428572</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.714285714285714</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.909090909090909</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.416666666666666</c:v>
+                  <c:v>2.083333333333333</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.461538461538461</c:v>
+                  <c:v>4.076923076923076</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9758,11 +9758,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2082189528"/>
-        <c:axId val="-2082287352"/>
+        <c:axId val="-2090227976"/>
+        <c:axId val="-2081676424"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2082189528"/>
+        <c:axId val="-2090227976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9797,7 +9797,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2082287352"/>
+        <c:crossAx val="-2081676424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9807,7 +9807,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2082287352"/>
+        <c:axId val="-2081676424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9852,7 +9852,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2082189528"/>
+        <c:crossAx val="-2090227976"/>
         <c:crossesAt val="1.0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10687,11 +10687,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2082252040"/>
-        <c:axId val="-2082248632"/>
+        <c:axId val="-2085400680"/>
+        <c:axId val="-2085406056"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2082252040"/>
+        <c:axId val="-2085400680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10726,7 +10726,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2082248632"/>
+        <c:crossAx val="-2085406056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10736,7 +10736,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2082248632"/>
+        <c:axId val="-2085406056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10781,7 +10781,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2082252040"/>
+        <c:crossAx val="-2085400680"/>
         <c:crossesAt val="1.0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11236,11 +11236,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2082379672"/>
-        <c:axId val="-2082376264"/>
+        <c:axId val="-2080051752"/>
+        <c:axId val="-2080146712"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2082379672"/>
+        <c:axId val="-2080051752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11275,7 +11275,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2082376264"/>
+        <c:crossAx val="-2080146712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11285,7 +11285,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2082376264"/>
+        <c:axId val="-2080146712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11330,7 +11330,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2082379672"/>
+        <c:crossAx val="-2080051752"/>
         <c:crossesAt val="1.0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -14112,11 +14112,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A8:B8"/>
     <mergeCell ref="A13:C13"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A10:B10"/>
@@ -14125,6 +14120,11 @@
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A8:B8"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -14340,11 +14340,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A8:B8"/>
     <mergeCell ref="A13:C13"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A10:B10"/>
@@ -14353,6 +14348,11 @@
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A8:B8"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -15532,13 +15532,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A1:R1"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A2:R2"/>
-    <mergeCell ref="A4:B4"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A13:B13"/>
@@ -15550,6 +15543,13 @@
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A17:Q17"/>
     <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A1:R1"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A2:R2"/>
+    <mergeCell ref="A4:B4"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -16304,17 +16304,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A11:I11"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A10:I10"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A11:I11"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A10:I10"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -16684,11 +16684,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A8:B8"/>
     <mergeCell ref="A13:C13"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A10:B10"/>
@@ -16697,6 +16692,11 @@
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A8:B8"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -16912,11 +16912,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A8:B8"/>
     <mergeCell ref="A13:C13"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A10:B10"/>
@@ -16925,6 +16920,11 @@
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A8:B8"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -19253,13 +19253,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A1:R1"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A2:R2"/>
-    <mergeCell ref="A4:B4"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A13:B13"/>
@@ -19271,6 +19264,13 @@
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A17:Q17"/>
     <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A1:R1"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A2:R2"/>
+    <mergeCell ref="A4:B4"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -20010,16 +20010,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A10:I10"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A9:I9"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -20037,12 +20037,12 @@
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
-    <tabColor theme="9"/>
+    <tabColor theme="2" tint="-0.749992370372631"/>
   </sheetPr>
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:J1"/>
+      <selection activeCell="L57" sqref="L57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -20236,11 +20236,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A8:B8"/>
     <mergeCell ref="A13:C13"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A10:B10"/>
@@ -20249,6 +20244,11 @@
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A8:B8"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -20464,11 +20464,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A8:B8"/>
     <mergeCell ref="A13:C13"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A10:B10"/>
@@ -20477,6 +20472,11 @@
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A8:B8"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -22826,13 +22826,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A1:R1"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A2:R2"/>
-    <mergeCell ref="A4:B4"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A13:B13"/>
@@ -22844,6 +22837,13 @@
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A17:Q17"/>
     <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A1:R1"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A2:R2"/>
+    <mergeCell ref="A4:B4"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -23346,8 +23346,8 @@
   </sheetPr>
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:I10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -23480,7 +23480,7 @@
       </c>
       <c r="I4" s="8">
         <f>((C4*C$11)+(D4*$D$11)+(E4*E11)+(F4*$F$11)+(G4*$G$11))/SUM(C4:G4)</f>
-        <v>3.4285714285714284</v>
+        <v>2.5714285714285716</v>
       </c>
       <c r="J4" s="3">
         <v>15</v>
@@ -23513,7 +23513,7 @@
       </c>
       <c r="I5" s="8">
         <f t="shared" ref="I5:I8" si="0">((C5*C$11)+(D5*$D$11)+(E5*E12)+(F5*$F$11)+(G5*$G$11))/SUM(C5:G5)</f>
-        <v>1.7142857142857142</v>
+        <v>3</v>
       </c>
       <c r="J5" s="3">
         <v>15</v>
@@ -23546,7 +23546,7 @@
       </c>
       <c r="I6" s="8">
         <f t="shared" si="0"/>
-        <v>3.9090909090909092</v>
+        <v>1</v>
       </c>
       <c r="J6" s="3">
         <v>15</v>
@@ -23579,7 +23579,7 @@
       </c>
       <c r="I7" s="8">
         <f t="shared" si="0"/>
-        <v>2.4166666666666665</v>
+        <v>2.0833333333333335</v>
       </c>
       <c r="J7" s="3">
         <v>15</v>
@@ -23612,7 +23612,7 @@
       </c>
       <c r="I8" s="8">
         <f t="shared" si="0"/>
-        <v>1.4615384615384615</v>
+        <v>4.0769230769230766</v>
       </c>
       <c r="J8" s="3">
         <v>14</v>
@@ -23684,33 +23684,33 @@
     </row>
     <row r="11" spans="1:10">
       <c r="C11" s="31">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D11" s="31">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E11" s="31">
         <v>3</v>
       </c>
       <c r="F11" s="31">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G11" s="31">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A10:I10"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A9:I9"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -24120,11 +24120,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A8:B8"/>
     <mergeCell ref="A13:C13"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A10:B10"/>
@@ -24133,6 +24128,11 @@
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A8:B8"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -24351,11 +24351,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A8:B8"/>
     <mergeCell ref="A13:C13"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A10:B10"/>
@@ -24364,6 +24359,11 @@
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A8:B8"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -25549,13 +25549,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A1:R1"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A2:R2"/>
-    <mergeCell ref="A4:B4"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A13:B13"/>
@@ -25567,6 +25560,13 @@
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A17:Q17"/>
     <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A1:R1"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A2:R2"/>
+    <mergeCell ref="A4:B4"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -25743,7 +25743,7 @@
   </sheetPr>
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
@@ -26137,17 +26137,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A11:I11"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A10:I10"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A11:I11"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A10:I10"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
FIX: Updated the exel spread sheet,
Question 54's weighting has been reversed

The tab color on Question 45 has been corrected.
</commit_message>
<xml_diff>
--- a/survey_data/SurveySummary_08192016.xlsx
+++ b/survey_data/SurveySummary_08192016.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="100" windowWidth="33240" windowHeight="19200" tabRatio="768" firstSheet="5" activeTab="8"/>
+    <workbookView xWindow="240" yWindow="100" windowWidth="33240" windowHeight="19200" tabRatio="768" firstSheet="24" activeTab="36"/>
   </bookViews>
   <sheets>
     <sheet name="Survey Tree Map" sheetId="56" r:id="rId1"/>
@@ -2062,11 +2062,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2079823976"/>
-        <c:axId val="-2080054952"/>
+        <c:axId val="-2073640872"/>
+        <c:axId val="-2073657736"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2079823976"/>
+        <c:axId val="-2073640872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2101,7 +2101,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2080054952"/>
+        <c:crossAx val="-2073657736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2111,7 +2111,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2080054952"/>
+        <c:axId val="-2073657736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2156,7 +2156,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2079823976"/>
+        <c:crossAx val="-2073640872"/>
         <c:crossesAt val="1.0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2865,11 +2865,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2092933080"/>
-        <c:axId val="-2075862952"/>
+        <c:axId val="-2073939736"/>
+        <c:axId val="-2073943128"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2092933080"/>
+        <c:axId val="-2073939736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2904,7 +2904,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2075862952"/>
+        <c:crossAx val="-2073943128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2914,7 +2914,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2075862952"/>
+        <c:axId val="-2073943128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2959,7 +2959,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2092933080"/>
+        <c:crossAx val="-2073939736"/>
         <c:crossesAt val="1.0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5208,11 +5208,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2081853208"/>
-        <c:axId val="-2081909496"/>
+        <c:axId val="-2085839896"/>
+        <c:axId val="-2085866456"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2081853208"/>
+        <c:axId val="-2085839896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5247,7 +5247,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2081909496"/>
+        <c:crossAx val="-2085866456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5257,7 +5257,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2081909496"/>
+        <c:axId val="-2085866456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5302,7 +5302,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2081853208"/>
+        <c:crossAx val="-2085839896"/>
         <c:crossesAt val="1.0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5545,11 +5545,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2085867032"/>
-        <c:axId val="-2080293000"/>
+        <c:axId val="-2086320968"/>
+        <c:axId val="-2086364184"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2085867032"/>
+        <c:axId val="-2086320968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5584,7 +5584,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2080293000"/>
+        <c:crossAx val="-2086364184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5594,7 +5594,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2080293000"/>
+        <c:axId val="-2086364184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5639,7 +5639,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2085867032"/>
+        <c:crossAx val="-2086320968"/>
         <c:crossesAt val="1.0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5822,11 +5822,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2096040632"/>
-        <c:axId val="-2086365416"/>
+        <c:axId val="-2086496440"/>
+        <c:axId val="-2086503704"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2096040632"/>
+        <c:axId val="-2086496440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5861,7 +5861,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2086365416"/>
+        <c:crossAx val="-2086503704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5871,7 +5871,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2086365416"/>
+        <c:axId val="-2086503704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5916,7 +5916,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2096040632"/>
+        <c:crossAx val="-2086496440"/>
         <c:crossesAt val="1.0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6386,11 +6386,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2076630808"/>
-        <c:axId val="-2076607880"/>
+        <c:axId val="-2087289720"/>
+        <c:axId val="-2087102792"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2076630808"/>
+        <c:axId val="-2087289720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6425,7 +6425,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2076607880"/>
+        <c:crossAx val="-2087102792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6435,7 +6435,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2076607880"/>
+        <c:axId val="-2087102792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6480,7 +6480,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2076630808"/>
+        <c:crossAx val="-2087289720"/>
         <c:crossesAt val="1.0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8580,11 +8580,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2079347640"/>
-        <c:axId val="-2080064328"/>
+        <c:axId val="-2090134440"/>
+        <c:axId val="-2082330056"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2079347640"/>
+        <c:axId val="-2090134440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8619,7 +8619,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2080064328"/>
+        <c:crossAx val="-2082330056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8629,7 +8629,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2080064328"/>
+        <c:axId val="-2082330056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8674,7 +8674,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2079347640"/>
+        <c:crossAx val="-2090134440"/>
         <c:crossesAt val="1.0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8917,11 +8917,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2082123448"/>
-        <c:axId val="-2082120024"/>
+        <c:axId val="-2087633896"/>
+        <c:axId val="-2081841944"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2082123448"/>
+        <c:axId val="-2087633896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8956,7 +8956,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2082120024"/>
+        <c:crossAx val="-2081841944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8966,7 +8966,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2082120024"/>
+        <c:axId val="-2081841944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9011,7 +9011,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2082123448"/>
+        <c:crossAx val="-2087633896"/>
         <c:crossesAt val="1.0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9194,11 +9194,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2082079320"/>
-        <c:axId val="-2082075928"/>
+        <c:axId val="-2082378664"/>
+        <c:axId val="-2082387976"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2082079320"/>
+        <c:axId val="-2082378664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9233,7 +9233,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2082075928"/>
+        <c:crossAx val="-2082387976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9243,7 +9243,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2082075928"/>
+        <c:axId val="-2082387976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9288,7 +9288,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2082079320"/>
+        <c:crossAx val="-2082378664"/>
         <c:crossesAt val="1.0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9731,19 +9731,19 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>3.428571428571428</c:v>
+                  <c:v>2.571428571428572</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.714285714285714</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.909090909090909</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.416666666666666</c:v>
+                  <c:v>2.083333333333333</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.461538461538461</c:v>
+                  <c:v>4.076923076923076</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9758,11 +9758,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2082189528"/>
-        <c:axId val="-2082287352"/>
+        <c:axId val="-2090227976"/>
+        <c:axId val="-2081676424"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2082189528"/>
+        <c:axId val="-2090227976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9797,7 +9797,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2082287352"/>
+        <c:crossAx val="-2081676424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9807,7 +9807,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2082287352"/>
+        <c:axId val="-2081676424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9852,7 +9852,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2082189528"/>
+        <c:crossAx val="-2090227976"/>
         <c:crossesAt val="1.0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10687,11 +10687,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2082252040"/>
-        <c:axId val="-2082248632"/>
+        <c:axId val="-2085400680"/>
+        <c:axId val="-2085406056"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2082252040"/>
+        <c:axId val="-2085400680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10726,7 +10726,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2082248632"/>
+        <c:crossAx val="-2085406056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10736,7 +10736,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2082248632"/>
+        <c:axId val="-2085406056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10781,7 +10781,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2082252040"/>
+        <c:crossAx val="-2085400680"/>
         <c:crossesAt val="1.0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11236,11 +11236,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2082379672"/>
-        <c:axId val="-2082376264"/>
+        <c:axId val="-2080051752"/>
+        <c:axId val="-2080146712"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2082379672"/>
+        <c:axId val="-2080051752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11275,7 +11275,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2082376264"/>
+        <c:crossAx val="-2080146712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11285,7 +11285,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2082376264"/>
+        <c:axId val="-2080146712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11330,7 +11330,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2082379672"/>
+        <c:crossAx val="-2080051752"/>
         <c:crossesAt val="1.0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -14112,11 +14112,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A8:B8"/>
     <mergeCell ref="A13:C13"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A10:B10"/>
@@ -14125,6 +14120,11 @@
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A8:B8"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -14340,11 +14340,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A8:B8"/>
     <mergeCell ref="A13:C13"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A10:B10"/>
@@ -14353,6 +14348,11 @@
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A8:B8"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -15532,13 +15532,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A1:R1"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A2:R2"/>
-    <mergeCell ref="A4:B4"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A13:B13"/>
@@ -15550,6 +15543,13 @@
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A17:Q17"/>
     <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A1:R1"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A2:R2"/>
+    <mergeCell ref="A4:B4"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -16304,17 +16304,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A11:I11"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A10:I10"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A11:I11"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A10:I10"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -16684,11 +16684,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A8:B8"/>
     <mergeCell ref="A13:C13"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A10:B10"/>
@@ -16697,6 +16692,11 @@
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A8:B8"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -16912,11 +16912,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A8:B8"/>
     <mergeCell ref="A13:C13"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A10:B10"/>
@@ -16925,6 +16920,11 @@
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A8:B8"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -19253,13 +19253,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A1:R1"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A2:R2"/>
-    <mergeCell ref="A4:B4"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A13:B13"/>
@@ -19271,6 +19264,13 @@
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A17:Q17"/>
     <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A1:R1"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A2:R2"/>
+    <mergeCell ref="A4:B4"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -20010,16 +20010,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A10:I10"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A9:I9"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -20037,12 +20037,12 @@
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
-    <tabColor theme="9"/>
+    <tabColor theme="2" tint="-0.749992370372631"/>
   </sheetPr>
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:J1"/>
+      <selection activeCell="L57" sqref="L57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -20236,11 +20236,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A8:B8"/>
     <mergeCell ref="A13:C13"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A10:B10"/>
@@ -20249,6 +20244,11 @@
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A8:B8"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -20464,11 +20464,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A8:B8"/>
     <mergeCell ref="A13:C13"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A10:B10"/>
@@ -20477,6 +20472,11 @@
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A8:B8"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -22826,13 +22826,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A1:R1"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A2:R2"/>
-    <mergeCell ref="A4:B4"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A13:B13"/>
@@ -22844,6 +22837,13 @@
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A17:Q17"/>
     <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A1:R1"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A2:R2"/>
+    <mergeCell ref="A4:B4"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -23346,8 +23346,8 @@
   </sheetPr>
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:I10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -23480,7 +23480,7 @@
       </c>
       <c r="I4" s="8">
         <f>((C4*C$11)+(D4*$D$11)+(E4*E11)+(F4*$F$11)+(G4*$G$11))/SUM(C4:G4)</f>
-        <v>3.4285714285714284</v>
+        <v>2.5714285714285716</v>
       </c>
       <c r="J4" s="3">
         <v>15</v>
@@ -23513,7 +23513,7 @@
       </c>
       <c r="I5" s="8">
         <f t="shared" ref="I5:I8" si="0">((C5*C$11)+(D5*$D$11)+(E5*E12)+(F5*$F$11)+(G5*$G$11))/SUM(C5:G5)</f>
-        <v>1.7142857142857142</v>
+        <v>3</v>
       </c>
       <c r="J5" s="3">
         <v>15</v>
@@ -23546,7 +23546,7 @@
       </c>
       <c r="I6" s="8">
         <f t="shared" si="0"/>
-        <v>3.9090909090909092</v>
+        <v>1</v>
       </c>
       <c r="J6" s="3">
         <v>15</v>
@@ -23579,7 +23579,7 @@
       </c>
       <c r="I7" s="8">
         <f t="shared" si="0"/>
-        <v>2.4166666666666665</v>
+        <v>2.0833333333333335</v>
       </c>
       <c r="J7" s="3">
         <v>15</v>
@@ -23612,7 +23612,7 @@
       </c>
       <c r="I8" s="8">
         <f t="shared" si="0"/>
-        <v>1.4615384615384615</v>
+        <v>4.0769230769230766</v>
       </c>
       <c r="J8" s="3">
         <v>14</v>
@@ -23684,33 +23684,33 @@
     </row>
     <row r="11" spans="1:10">
       <c r="C11" s="31">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D11" s="31">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E11" s="31">
         <v>3</v>
       </c>
       <c r="F11" s="31">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G11" s="31">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A10:I10"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A9:I9"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -24120,11 +24120,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A8:B8"/>
     <mergeCell ref="A13:C13"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A10:B10"/>
@@ -24133,6 +24128,11 @@
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A8:B8"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -24351,11 +24351,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A8:B8"/>
     <mergeCell ref="A13:C13"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A10:B10"/>
@@ -24364,6 +24359,11 @@
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A8:B8"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -25549,13 +25549,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A1:R1"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A2:R2"/>
-    <mergeCell ref="A4:B4"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A13:B13"/>
@@ -25567,6 +25560,13 @@
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A17:Q17"/>
     <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A1:R1"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A2:R2"/>
+    <mergeCell ref="A4:B4"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -25743,7 +25743,7 @@
   </sheetPr>
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
@@ -26137,17 +26137,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A11:I11"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A10:I10"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A11:I11"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A10:I10"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>